<commit_message>
added CELL_NAMES for all columns
</commit_message>
<xml_diff>
--- a/market_price_data.xlsx
+++ b/market_price_data.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2979" uniqueCount="99">
   <si>
-    <t>date</t>
+    <t>Date</t>
   </si>
   <si>
-    <t>time</t>
+    <t>Time</t>
   </si>
   <si>
-    <t>market_price</t>
+    <t>Market_price</t>
   </si>
   <si>
     <t>00:00+01:00</t>

</xml_diff>